<commit_message>
A stub in the absence of a photo
</commit_message>
<xml_diff>
--- a/wine_new_2.xlsx
+++ b/wine_new_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilu/dev/wine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE866F8F-3232-624E-BA09-A39D5771EA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9711B3-140C-0D4E-BA3E-1B1213DF4C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Название</t>
   </si>
@@ -406,7 +406,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -595,9 +595,7 @@
       <c r="D11" s="2">
         <v>100</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -612,9 +610,7 @@
       <c r="D12" s="2">
         <v>150</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -629,9 +625,7 @@
       <c r="D13" s="2">
         <v>50</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>